<commit_message>
HW1 P6 tidy up data
</commit_message>
<xml_diff>
--- a/data/survey_data.xlsx
+++ b/data/survey_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trvrb/Documents/src/tfcb_2019/homeworks/homework01/messy-project-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carli\OneDrive\Documents\M3D\MCB536\tfcb-homework01\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A2EF31-99BB-1147-875E-0BF67F65B824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95290F78-B9D2-4B8B-B2F1-7E78FCC2232F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1400" windowWidth="25120" windowHeight="15580" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
     <sheet name="2014" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="41">
   <si>
     <t>NA</t>
   </si>
@@ -140,6 +141,18 @@
   </si>
   <si>
     <t>gray cell means my measurement device wasn't calibrated correctly</t>
+  </si>
+  <si>
+    <t>OL</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>Weight (g)</t>
+  </si>
+  <si>
+    <t>CollectionDate</t>
   </si>
 </sst>
 </file>
@@ -149,7 +162,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -187,6 +200,11 @@
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -317,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,17 +352,45 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
@@ -423,6 +469,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3FF7842C-E212-4893-B5C5-20818E5664DB}" name="Table2" displayName="Table2" ref="A1:E49" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E49" xr:uid="{3FF7842C-E212-4893-B5C5-20818E5664DB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E49">
+    <sortCondition ref="C1:C49"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F60C6E3E-B714-47A9-811B-A4F6EB8E6114}" name="Species" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{C5A49C75-38F8-43E5-A5D6-0E794D20D52F}" name="Plot"/>
+    <tableColumn id="3" xr3:uid="{3F80E61F-5F1A-4D39-A04D-130C0DD241B3}" name="CollectionDate"/>
+    <tableColumn id="4" xr3:uid="{61E98EFA-F760-487B-B141-B1073FE3C383}" name="Sex"/>
+    <tableColumn id="5" xr3:uid="{A282D65D-0E65-4219-81BE-7BBF7DCD6C6C}" name="Weight (g)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -731,7 +794,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -775,7 +838,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -799,31 +862,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:AB28"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="84" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="25" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="1"/>
-    <col min="3" max="3" width="26.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="24.83203125" customWidth="1"/>
-    <col min="16" max="16" width="52.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="1"/>
+    <col min="3" max="3" width="26.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.6328125" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.36328125" customWidth="1"/>
+    <col min="13" max="13" width="24.81640625" customWidth="1"/>
+    <col min="16" max="16" width="52.81640625" customWidth="1"/>
     <col min="17" max="17" width="18" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="1"/>
-    <col min="21" max="21" width="19.83203125" customWidth="1"/>
-    <col min="26" max="26" width="17.5" customWidth="1"/>
-    <col min="29" max="16384" width="11.5" style="1"/>
+    <col min="20" max="20" width="11.453125" style="1"/>
+    <col min="21" max="21" width="19.81640625" customWidth="1"/>
+    <col min="26" max="26" width="17.453125" customWidth="1"/>
+    <col min="29" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:17" ht="79" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:17" ht="79" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C3" s="11" t="s">
         <v>20</v>
       </c>
@@ -842,7 +905,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -859,7 +922,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -876,7 +939,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
@@ -899,298 +962,298 @@
       <c r="P6" s="14"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="P7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C8" s="18">
+    <row r="8" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" s="17">
         <v>41471</v>
       </c>
-      <c r="D8" s="16">
-        <v>2</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="17"/>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <v>41505</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="5">
         <v>8</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="17">
+      <c r="J8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="16">
         <v>52</v>
       </c>
       <c r="L8" s="5"/>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <v>41590</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="5">
         <v>9</v>
       </c>
-      <c r="O8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="17">
+      <c r="O8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="16">
         <v>117</v>
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C9" s="18">
+    <row r="9" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" s="17">
         <v>41471</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="5">
         <v>7</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <v>41564</v>
       </c>
-      <c r="I9" s="16">
-        <v>3</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="17">
+      <c r="I9" s="5">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="16">
         <v>33</v>
       </c>
       <c r="L9" s="5"/>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <v>41591</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="5">
         <v>11</v>
       </c>
-      <c r="O9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="17">
+      <c r="O9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="16">
         <v>126</v>
       </c>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C10" s="18">
+    <row r="10" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="17">
         <v>41471</v>
       </c>
-      <c r="D10" s="16">
-        <v>3</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="17"/>
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="18">
+      <c r="H10" s="17">
         <v>41564</v>
       </c>
-      <c r="I10" s="16">
-        <v>3</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="17">
+      <c r="I10" s="5">
+        <v>3</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="16">
         <v>50</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="M10" s="18">
+      <c r="M10" s="17">
         <v>41591</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="5">
         <v>17</v>
       </c>
-      <c r="O10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="P10" s="17" t="s">
+      <c r="O10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" s="16" t="s">
         <v>27</v>
       </c>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C11" s="18">
+    <row r="11" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="17">
         <v>41471</v>
       </c>
-      <c r="D11" s="16">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="17"/>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="16"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>41618</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="5">
         <v>9</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="17">
+      <c r="J11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="16">
         <v>40</v>
       </c>
       <c r="L11" s="5"/>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <v>41591</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N11" s="5">
         <v>14</v>
       </c>
-      <c r="O11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="17" t="s">
+      <c r="O11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C12" s="18">
+    <row r="12" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="17">
         <v>41473</v>
       </c>
-      <c r="D12" s="16">
-        <v>3</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="17" t="s">
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <v>41618</v>
       </c>
-      <c r="I12" s="16">
-        <v>1</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="17">
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="16">
         <v>45</v>
       </c>
       <c r="L12" s="5"/>
-      <c r="M12" s="18">
+      <c r="M12" s="17">
         <v>41591</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="5">
         <v>11</v>
       </c>
-      <c r="O12" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="17">
+      <c r="O12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="16">
         <v>122</v>
       </c>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C13" s="18">
+    <row r="13" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" s="17">
         <v>41473</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="5">
         <v>7</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17" t="s">
+      <c r="E13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <v>41619</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="19">
         <v>8</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="21">
+      <c r="J13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="20">
         <v>41</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="18">
+      <c r="M13" s="17">
         <v>41591</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="5">
         <v>4</v>
       </c>
-      <c r="O13" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P13" s="17">
+      <c r="O13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="16">
         <v>107</v>
       </c>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C14" s="18">
+    <row r="14" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" s="17">
         <v>41473</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="5">
         <v>4</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="E14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="5"/>
@@ -1199,31 +1262,31 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="19">
+      <c r="M14" s="18">
         <v>41591</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="19">
         <v>4</v>
       </c>
-      <c r="O14" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="P14" s="21">
+      <c r="O14" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" s="20">
         <v>115</v>
       </c>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C15" s="19">
+    <row r="15" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" s="18">
         <v>41473</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>6</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="21" t="s">
+      <c r="E15" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="5"/>
@@ -1238,7 +1301,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1255,7 +1318,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1272,7 +1335,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1289,7 +1352,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1306,7 +1369,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1323,7 +1386,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1340,7 +1403,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1357,7 +1420,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="G23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
@@ -1366,7 +1429,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="G24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
@@ -1375,22 +1438,22 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="G25" s="5"/>
       <c r="L25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="G26" s="5"/>
       <c r="L26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="G27" s="5"/>
       <c r="L27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="G28" s="5"/>
       <c r="L28" s="5"/>
       <c r="Q28" s="5"/>
@@ -1410,29 +1473,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView zoomScale="62" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="25" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="11.5" style="1"/>
-    <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" style="1" customWidth="1"/>
-    <col min="10" max="12" width="11.5" style="1"/>
-    <col min="13" max="13" width="22.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" style="1" customWidth="1"/>
-    <col min="15" max="19" width="11.5" style="1"/>
+    <col min="3" max="3" width="22.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1796875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="11.453125" style="1"/>
+    <col min="8" max="8" width="22.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" style="1" customWidth="1"/>
+    <col min="10" max="12" width="11.453125" style="1"/>
+    <col min="13" max="13" width="22.453125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.1796875" style="1" customWidth="1"/>
+    <col min="15" max="19" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:17" ht="69" customHeight="1" x14ac:dyDescent="0.7">
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
@@ -1455,7 +1518,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1496,7 +1559,7 @@
       </c>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="6">
         <v>41648</v>
       </c>
@@ -1520,7 +1583,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="5"/>
       <c r="M8" s="7">
-        <v>42074</v>
+        <v>45727</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>4</v>
@@ -1533,7 +1596,7 @@
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="6">
         <v>41648</v>
       </c>
@@ -1572,7 +1635,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" s="6">
         <v>41711</v>
       </c>
@@ -1607,7 +1670,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" s="6">
         <v>41711</v>
       </c>
@@ -1648,7 +1711,7 @@
       </c>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" s="6">
         <v>41711</v>
       </c>
@@ -1685,7 +1748,7 @@
       </c>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1718,7 +1781,7 @@
       </c>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1747,7 +1810,7 @@
       </c>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1772,7 +1835,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1797,7 +1860,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1822,7 +1885,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1839,7 +1902,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1856,7 +1919,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1873,7 +1936,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1890,7 +1953,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="3:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:17" ht="31" x14ac:dyDescent="0.7">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1909,7 +1972,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1926,7 +1989,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1943,7 +2006,7 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -1960,7 +2023,7 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -1977,7 +2040,7 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" s="4" t="s">
         <v>29</v>
       </c>
@@ -1996,7 +2059,7 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="4" t="s">
         <v>16</v>
       </c>
@@ -2019,7 +2082,7 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" s="6">
         <v>28498</v>
       </c>
@@ -2042,7 +2105,7 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" s="6">
         <v>28498</v>
       </c>
@@ -2063,7 +2126,7 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C31" s="6">
         <v>28498</v>
       </c>
@@ -2086,7 +2149,7 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="6">
         <v>28498</v>
       </c>
@@ -2109,7 +2172,7 @@
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C33" s="6">
         <v>28498</v>
       </c>
@@ -2132,7 +2195,7 @@
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -2149,7 +2212,7 @@
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
     </row>
-    <row r="35" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -2166,7 +2229,7 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -2183,7 +2246,7 @@
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -2198,7 +2261,7 @@
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -2215,7 +2278,7 @@
       <c r="P38" s="5"/>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="L39" s="5"/>
@@ -2225,7 +2288,7 @@
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="L40" s="5"/>
@@ -2235,7 +2298,7 @@
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
     </row>
-    <row r="41" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="L41" s="5"/>
@@ -2245,34 +2308,34 @@
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="L42" s="5"/>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="L43" s="5"/>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="G44" s="5"/>
       <c r="L44" s="5"/>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="G45" s="5"/>
       <c r="L45" s="5"/>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="G46" s="5"/>
       <c r="L46" s="5"/>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:17" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="G47" s="5"/>
       <c r="L47" s="5"/>
       <c r="Q47" s="5"/>
@@ -2280,10 +2343,868 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C351A05-D9A7-4039-9471-908F5C4C9900}">
+  <dimension ref="A1:E50"/>
+  <sheetViews>
+    <sheetView zoomScale="122" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>19780108</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>19780108</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>19780108</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>19780108</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>19780108</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>20130716</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>20130716</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>20130716</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>20130716</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>20130718</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>20130718</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>20130718</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>20130718</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>20130819</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>20131017</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>20131017</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>20131112</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>20131113</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>20131113</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>20131113</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>20131113</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>20131113</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>20131113</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>20131210</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>20131210</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>20131211</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>20140108</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>20140108</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>20140108</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>20140108</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>20140108</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>20140108</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>20140108</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>20140109</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>20140109</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>20140218</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>20140218</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>20140218</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>20140313</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>20140313</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>20140313</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>20140408</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>20140506</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>20140518</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>20140609</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>20140708</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>20140708</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>20141103</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>